<commit_message>
make ASN 2023 poster
</commit_message>
<xml_diff>
--- a/eg_data/NHANES/PF/20_BMI.xlsx
+++ b/eg_data/NHANES/PF/20_BMI.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sadoh\OneDrive\Documents\GitHub\DietR\eg_data\NHANES\PF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5AE0321-28DB-453E-A66E-476703B3152A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C188C9-47F1-4426-A1FB-997A5057AF01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30915" yWindow="-3360" windowWidth="18240" windowHeight="15615" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="62">
   <si>
     <t>With Gender &amp; Age</t>
   </si>
@@ -409,6 +412,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFDCBCB"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -418,6 +426,1046 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.217186428229593"/>
+          <c:y val="6.7276620684465105E-2"/>
+          <c:w val="0.74713790216847809"/>
+          <c:h val="0.76845122306270808"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$T$149</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>emmean</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FDCBCB"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$D$160:$D$163</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>0.165029993120519</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.198631664864556</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.36657527711677601</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.37673361200355499</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$D$160:$D$163</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>0.165029993120519</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.198631664864556</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.36657527711677601</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.37673361200355499</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$S$150:$S$153</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>DivNA</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Div0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Div1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Div2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$T$150:$T$153</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>29.833039894761601</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29.701989237987501</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>28.923320343383399</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>27.695775047685299</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-503C-48A4-9927-02EDC1D3386F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="149"/>
+        <c:overlap val="-45"/>
+        <c:axId val="477875424"/>
+        <c:axId val="477873624"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="477875424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="65000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="477873624"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="477873624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="477875424"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="65000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1600">
+          <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId3"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>148</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>232834</xdr:colOff>
+      <xdr:row>162</xdr:row>
+      <xdr:rowOff>52916</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D535927-A1F8-4FFC-A1B7-6297A959B02A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>2.55373E-7</cdr:x>
+      <cdr:y>0.01167</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.1</cdr:x>
+      <cdr:y>0.89883</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{855F7DC9-3DD0-48DB-EA7D-4FA42F8645E7}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="16200000">
+          <a:off x="-1010712" y="1042454"/>
+          <a:ext cx="2413009" cy="391583"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>BMI</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1050">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Waist"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="185">
+          <cell r="T185" t="str">
+            <v>Waist</v>
+          </cell>
+        </row>
+        <row r="186">
+          <cell r="D186">
+            <v>0.38875277517771301</v>
+          </cell>
+          <cell r="S186" t="str">
+            <v>DivNA</v>
+          </cell>
+          <cell r="T186">
+            <v>101.209878392053</v>
+          </cell>
+        </row>
+        <row r="187">
+          <cell r="D187">
+            <v>0.46790652713579101</v>
+          </cell>
+          <cell r="S187" t="str">
+            <v>Div0</v>
+          </cell>
+          <cell r="T187">
+            <v>100.482176745179</v>
+          </cell>
+        </row>
+        <row r="188">
+          <cell r="D188">
+            <v>0.86352276695918195</v>
+          </cell>
+          <cell r="S188" t="str">
+            <v>Div1</v>
+          </cell>
+          <cell r="T188">
+            <v>99.029510455848794</v>
+          </cell>
+        </row>
+        <row r="189">
+          <cell r="D189">
+            <v>0.88745224064907202</v>
+          </cell>
+          <cell r="S189" t="str">
+            <v>Div2</v>
+          </cell>
+          <cell r="T189">
+            <v>95.9339848387296</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -683,10 +1731,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q172"/>
+  <dimension ref="A1:T172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J143" sqref="J143"/>
+    <sheetView tabSelected="1" topLeftCell="A150" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I164" sqref="I164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3898,22 +4946,22 @@
         <v>43</v>
       </c>
     </row>
-    <row r="145" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:20" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A145" s="29" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="146" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:20" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A146" s="29" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="147" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="149" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B149" s="2"/>
       <c r="C149" s="2" t="s">
         <v>32</v>
@@ -3940,8 +4988,14 @@
       <c r="O149" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="150" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S149" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="T149" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="150" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B150" t="s">
         <v>36</v>
       </c>
@@ -3970,11 +5024,17 @@
         <v>4324.2979628871599</v>
       </c>
       <c r="O150" s="46" t="str">
-        <f t="shared" ref="O150:O155" si="4">IF(F150&lt;0.0001,"&lt;0.0001",IF(F150&lt;0.001,"&lt;0.001",IF(F150&lt;0.01,"&lt;0.01",ROUND(F150,3))))</f>
+        <f t="shared" ref="O150:O154" si="4">IF(F150&lt;0.0001,"&lt;0.0001",IF(F150&lt;0.001,"&lt;0.001",IF(F150&lt;0.01,"&lt;0.01",ROUND(F150,3))))</f>
         <v>&lt;0.0001</v>
       </c>
-    </row>
-    <row r="151" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S150" t="s">
+        <v>3</v>
+      </c>
+      <c r="T150" s="3">
+        <v>29.833039894761601</v>
+      </c>
+    </row>
+    <row r="151" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B151" t="s">
         <v>2</v>
       </c>
@@ -4006,8 +5066,14 @@
         <f t="shared" si="4"/>
         <v>&lt;0.0001</v>
       </c>
-    </row>
-    <row r="152" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S151" t="s">
+        <v>4</v>
+      </c>
+      <c r="T151" s="3">
+        <v>29.701989237987501</v>
+      </c>
+    </row>
+    <row r="152" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
         <v>37</v>
       </c>
@@ -4039,8 +5105,14 @@
         <f t="shared" si="4"/>
         <v>&lt;0.0001</v>
       </c>
-    </row>
-    <row r="153" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S152" t="s">
+        <v>5</v>
+      </c>
+      <c r="T152" s="3">
+        <v>28.923320343383399</v>
+      </c>
+    </row>
+    <row r="153" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B153" t="s">
         <v>38</v>
       </c>
@@ -4072,8 +5144,14 @@
         <f t="shared" si="4"/>
         <v>&lt;0.0001</v>
       </c>
-    </row>
-    <row r="154" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S153" t="s">
+        <v>6</v>
+      </c>
+      <c r="T153" s="3">
+        <v>27.695775047685299</v>
+      </c>
+    </row>
+    <row r="154" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B154" t="s">
         <v>44</v>
       </c>
@@ -4106,7 +5184,7 @@
         <v>&lt;0.001</v>
       </c>
     </row>
-    <row r="155" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
         <v>51</v>
       </c>
@@ -4139,7 +5217,7 @@
         <v>&lt;0.0001</v>
       </c>
     </row>
-    <row r="156" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B156" s="2" t="s">
         <v>40</v>
       </c>
@@ -4171,7 +5249,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="159" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
         <v>2</v>
       </c>
@@ -4221,7 +5299,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="160" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>3</v>
       </c>
@@ -4740,5 +5818,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>